<commit_message>
Update data files and scripts - 2026-02-11
Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/nifty_options/nifty_options_2026-02.xlsx
+++ b/data/nifty_options/nifty_options_2026-02.xlsx
@@ -478,7 +478,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE5"/>
+  <dimension ref="A1:AE8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1145,6 +1145,357 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-09</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>10:00:13</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="D6" s="4" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="inlineStr">
+        <is>
+          <t>TRADEABLE</t>
+        </is>
+      </c>
+      <c r="G6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="6" t="n">
+        <v>25814.7</v>
+      </c>
+      <c r="I6" s="6" t="n">
+        <v>12.15</v>
+      </c>
+      <c r="J6" s="6" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="K6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" s="5" t="n">
+        <v>43.1</v>
+      </c>
+      <c r="M6" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="N6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="P6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" s="2" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="U6" s="2" t="inlineStr"/>
+      <c r="V6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="2" t="inlineStr">
+        <is>
+          <t>HARD VETO: CPR TRENDING DAY: Price 25814.70 above TC 25661.78 - BULLISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AD6" s="2" t="inlineStr">
+        <is>
+          <t>CPR TRENDING DAY: Price 25814.70 above TC 25661.78 - BULLISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AE6" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-10</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>10:00:10</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="D7" s="4" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="inlineStr">
+        <is>
+          <t>TRADEABLE</t>
+        </is>
+      </c>
+      <c r="G7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="6" t="n">
+        <v>25949.95</v>
+      </c>
+      <c r="I7" s="6" t="n">
+        <v>11.95</v>
+      </c>
+      <c r="J7" s="6" t="n">
+        <v>-0.22</v>
+      </c>
+      <c r="K7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="5" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="M7" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="N7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="P7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" s="2" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="U7" s="2" t="inlineStr"/>
+      <c r="V7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="2" t="inlineStr">
+        <is>
+          <t>HARD VETO: CPR TRENDING DAY: Price 25949.95 above TC 25862.06 - BULLISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AD7" s="2" t="inlineStr">
+        <is>
+          <t>CPR TRENDING DAY: Price 25949.95 above TC 25862.06 - BULLISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AE7" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-11</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>10:00:08</t>
+        </is>
+      </c>
+      <c r="C8" s="3" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="D8" s="4" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="E8" s="2" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="inlineStr">
+        <is>
+          <t>TRADEABLE</t>
+        </is>
+      </c>
+      <c r="G8" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="6" t="n">
+        <v>25943.05</v>
+      </c>
+      <c r="I8" s="6" t="n">
+        <v>11.54</v>
+      </c>
+      <c r="J8" s="6" t="n">
+        <v>-0.4</v>
+      </c>
+      <c r="K8" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" s="5" t="n">
+        <v>29.3</v>
+      </c>
+      <c r="M8" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="N8" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="P8" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R8" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" s="2" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="U8" s="2" t="inlineStr"/>
+      <c r="V8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W8" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X8" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="2" t="inlineStr">
+        <is>
+          <t>HARD VETO: CPR TRENDING DAY: Price 25943.05 above TC 25933.42 - BULLISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AD8" s="2" t="inlineStr">
+        <is>
+          <t>CPR TRENDING DAY: Price 25943.05 above TC 25933.42 - BULLISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AE8" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix early_warning poisoning rapid alert cooldowns & add backtest scripts
The early_warning_detector's _should_send_prealert() used should_send_alert()
to check for recent 5-min alerts, but that method has a side effect of recording
the current time. This poisoned the cooldown for the actual rapid_drop_detector,
silencing 11 out of 12 alerts on Feb 17. Fixed by using the read-only
get_last_alert_time() instead.

Also adds post-noon backtest scripts for 5-min alerts and pre-alerts.

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/nifty_options/nifty_options_2026-02.xlsx
+++ b/data/nifty_options/nifty_options_2026-02.xlsx
@@ -478,7 +478,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE8"/>
+  <dimension ref="A1:AE12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1496,6 +1496,474 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-13</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>10:00:10</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="D9" s="4" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="F9" s="2" t="inlineStr">
+        <is>
+          <t>TRADEABLE</t>
+        </is>
+      </c>
+      <c r="G9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="6" t="n">
+        <v>25536</v>
+      </c>
+      <c r="I9" s="6" t="n">
+        <v>12.27</v>
+      </c>
+      <c r="J9" s="6" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="K9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="5" t="n">
+        <v>48</v>
+      </c>
+      <c r="M9" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="N9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="P9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T9" s="2" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="U9" s="2" t="inlineStr"/>
+      <c r="V9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="2" t="inlineStr">
+        <is>
+          <t>HARD VETO: CPR TRENDING DAY: Price 25536.00 below BC 25829.55 - BEARISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AD9" s="2" t="inlineStr">
+        <is>
+          <t>CPR TRENDING DAY: Price 25536.00 below BC 25829.55 - BEARISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AE9" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-16</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>10:00:10</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="D10" s="4" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="inlineStr">
+        <is>
+          <t>TRADEABLE</t>
+        </is>
+      </c>
+      <c r="G10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="6" t="n">
+        <v>25498.35</v>
+      </c>
+      <c r="I10" s="6" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="J10" s="6" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="K10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="5" t="n">
+        <v>61</v>
+      </c>
+      <c r="M10" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="N10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="P10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T10" s="2" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="U10" s="2" t="inlineStr"/>
+      <c r="V10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="2" t="inlineStr">
+        <is>
+          <t>HARD VETO: CPR TRENDING DAY: Price 25498.35 above TC 25493.18 - BULLISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AD10" s="2" t="inlineStr">
+        <is>
+          <t>CPR TRENDING DAY: Price 25498.35 above TC 25493.18 - BULLISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AE10" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-17</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>10:00:08</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="D11" s="4" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="inlineStr">
+        <is>
+          <t>TRADEABLE</t>
+        </is>
+      </c>
+      <c r="G11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="6" t="n">
+        <v>25661.75</v>
+      </c>
+      <c r="I11" s="6" t="n">
+        <v>13.06</v>
+      </c>
+      <c r="J11" s="6" t="n">
+        <v>1.33</v>
+      </c>
+      <c r="K11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" s="5" t="n">
+        <v>56.9</v>
+      </c>
+      <c r="M11" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="N11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O11" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="P11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T11" s="2" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="U11" s="2" t="inlineStr"/>
+      <c r="V11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W11" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X11" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="2" t="inlineStr">
+        <is>
+          <t>HARD VETO: CPR TRENDING DAY: Price 25661.75 above TC 25633.45 - BULLISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AD11" s="2" t="inlineStr">
+        <is>
+          <t>CPR TRENDING DAY: Price 25661.75 above TC 25633.45 - BULLISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AE11" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-18</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>10:00:11</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="D12" s="4" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="inlineStr">
+        <is>
+          <t>TRADEABLE</t>
+        </is>
+      </c>
+      <c r="G12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="6" t="n">
+        <v>25666.7</v>
+      </c>
+      <c r="I12" s="6" t="n">
+        <v>12.58</v>
+      </c>
+      <c r="J12" s="6" t="n">
+        <v>-0.71</v>
+      </c>
+      <c r="K12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" s="5" t="n">
+        <v>53</v>
+      </c>
+      <c r="M12" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="N12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="P12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T12" s="2" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="U12" s="2" t="inlineStr"/>
+      <c r="V12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W12" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X12" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="2" t="inlineStr">
+        <is>
+          <t>HARD VETO: CPR TRENDING DAY: Price 25666.70 below BC 25667.35 - BEARISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AD12" s="2" t="inlineStr">
+        <is>
+          <t>CPR TRENDING DAY: Price 25666.70 below BC 25667.35 - BEARISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AE12" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update data files - 2026-02-19
Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/nifty_options/nifty_options_2026-02.xlsx
+++ b/data/nifty_options/nifty_options_2026-02.xlsx
@@ -478,7 +478,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE12"/>
+  <dimension ref="A1:AE13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1964,6 +1964,123 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-19</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>10:00:13</t>
+        </is>
+      </c>
+      <c r="C13" s="3" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="D13" s="4" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="F13" s="2" t="inlineStr">
+        <is>
+          <t>TRADEABLE</t>
+        </is>
+      </c>
+      <c r="G13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="6" t="n">
+        <v>25773.7</v>
+      </c>
+      <c r="I13" s="6" t="n">
+        <v>12.21</v>
+      </c>
+      <c r="J13" s="6" t="n">
+        <v>-1.12</v>
+      </c>
+      <c r="K13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" s="5" t="n">
+        <v>46.5</v>
+      </c>
+      <c r="M13" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="N13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="P13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T13" s="2" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="U13" s="2" t="inlineStr"/>
+      <c r="V13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W13" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X13" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="2" t="inlineStr">
+        <is>
+          <t>HARD VETO: CPR TRENDING DAY: Price 25773.70 within CPR (25736.60 - 25791.77) - SIDEWAYS/RANGE-BOUND BUT VERY NARROW CPR (0.214%) suggests trending day</t>
+        </is>
+      </c>
+      <c r="AD13" s="2" t="inlineStr">
+        <is>
+          <t>CPR TRENDING DAY: Price 25773.70 within CPR (25736.60 - 25791.77) - SIDEWAYS/RANGE-BOUND BUT VERY NARROW CPR (0.214%) suggests trending day</t>
+        </is>
+      </c>
+      <c r="AE13" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update data files and scripts - 2026-02-26
Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/nifty_options/nifty_options_2026-02.xlsx
+++ b/data/nifty_options/nifty_options_2026-02.xlsx
@@ -478,7 +478,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE13"/>
+  <dimension ref="A1:AE17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2081,6 +2081,474 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>10:00:09</t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="D14" s="4" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="F14" s="2" t="inlineStr">
+        <is>
+          <t>TRADEABLE</t>
+        </is>
+      </c>
+      <c r="G14" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="6" t="n">
+        <v>25522.2</v>
+      </c>
+      <c r="I14" s="6" t="n">
+        <v>14.18</v>
+      </c>
+      <c r="J14" s="6" t="n">
+        <v>1.51</v>
+      </c>
+      <c r="K14" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" s="5" t="n">
+        <v>73.09999999999999</v>
+      </c>
+      <c r="M14" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="N14" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="P14" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R14" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S14" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T14" s="2" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="U14" s="2" t="inlineStr"/>
+      <c r="V14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W14" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X14" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="2" t="inlineStr">
+        <is>
+          <t>HARD VETO: CPR TRENDING DAY: Price 25522.20 above TC 25515.24 - BULLISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AD14" s="2" t="inlineStr">
+        <is>
+          <t>CPR TRENDING DAY: Price 25522.20 above TC 25515.24 - BULLISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AE14" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-23</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>10:00:12</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="D15" s="4" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="F15" s="2" t="inlineStr">
+        <is>
+          <t>TRADEABLE</t>
+        </is>
+      </c>
+      <c r="G15" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="6" t="n">
+        <v>25728.75</v>
+      </c>
+      <c r="I15" s="6" t="n">
+        <v>14.23</v>
+      </c>
+      <c r="J15" s="6" t="n">
+        <v>2.01</v>
+      </c>
+      <c r="K15" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" s="5" t="n">
+        <v>74.3</v>
+      </c>
+      <c r="M15" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="N15" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="P15" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R15" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S15" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T15" s="2" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="U15" s="2" t="inlineStr"/>
+      <c r="V15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="2" t="inlineStr">
+        <is>
+          <t>HARD VETO: CPR TRENDING DAY: Price 25728.75 above TC 25554.72 - BULLISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AD15" s="2" t="inlineStr">
+        <is>
+          <t>CPR TRENDING DAY: Price 25728.75 above TC 25554.72 - BULLISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AE15" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-24</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="inlineStr">
+        <is>
+          <t>10:00:12</t>
+        </is>
+      </c>
+      <c r="C16" s="3" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="D16" s="4" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="F16" s="2" t="inlineStr">
+        <is>
+          <t>TRADEABLE</t>
+        </is>
+      </c>
+      <c r="G16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="6" t="n">
+        <v>25516.75</v>
+      </c>
+      <c r="I16" s="6" t="n">
+        <v>14</v>
+      </c>
+      <c r="J16" s="6" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="K16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" s="5" t="n">
+        <v>71</v>
+      </c>
+      <c r="M16" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="N16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="P16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T16" s="2" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="U16" s="2" t="inlineStr"/>
+      <c r="V16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W16" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X16" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="2" t="inlineStr">
+        <is>
+          <t>HARD VETO: CPR TRENDING DAY: Price 25516.75 below BC 25690.40 - BEARISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AD16" s="2" t="inlineStr">
+        <is>
+          <t>CPR TRENDING DAY: Price 25516.75 below BC 25690.40 - BEARISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AE16" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>2026-02-25</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="inlineStr">
+        <is>
+          <t>10:00:12</t>
+        </is>
+      </c>
+      <c r="C17" s="3" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="D17" s="4" t="inlineStr">
+        <is>
+          <t>AVOID</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="F17" s="2" t="inlineStr">
+        <is>
+          <t>TRADEABLE</t>
+        </is>
+      </c>
+      <c r="G17" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="6" t="n">
+        <v>25600.15</v>
+      </c>
+      <c r="I17" s="6" t="n">
+        <v>13.07</v>
+      </c>
+      <c r="J17" s="6" t="n">
+        <v>-1.29</v>
+      </c>
+      <c r="K17" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" s="5" t="n">
+        <v>57</v>
+      </c>
+      <c r="M17" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="N17" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O17" s="2" t="inlineStr">
+        <is>
+          <t>UNKNOWN</t>
+        </is>
+      </c>
+      <c r="P17" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R17" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S17" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T17" s="2" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="U17" s="2" t="inlineStr"/>
+      <c r="V17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="2" t="inlineStr">
+        <is>
+          <t>HARD VETO: CPR TRENDING DAY: Price 25600.15 above TC 25444.67 - BULLISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AD17" s="2" t="inlineStr">
+        <is>
+          <t>CPR TRENDING DAY: Price 25600.15 above TC 25444.67 - BULLISH TRENDING DAY likely</t>
+        </is>
+      </c>
+      <c r="AE17" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>